<commit_message>
Converted BOM and updated Schematics and Board
</commit_message>
<xml_diff>
--- a/Notes/Pogo BOM.xlsx
+++ b/Notes/Pogo BOM.xlsx
@@ -1,25 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="150" windowWidth="24240" windowHeight="12075"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Electronics" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="Goal">Sheet1!$K$1</definedName>
+    <definedName name="Goal">Electronics!$K$1</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t>Mfg Part #</t>
   </si>
@@ -64,6 +62,24 @@
   </si>
   <si>
     <t>Bill of Materials - Pogo</t>
+  </si>
+  <si>
+    <t>68021-106HLF</t>
+  </si>
+  <si>
+    <t>CONN HEADER 6POS (2x3) Right Angle</t>
+  </si>
+  <si>
+    <t>CONN HEADER 10POS (2x5) Right Angle</t>
+  </si>
+  <si>
+    <t>.100"</t>
+  </si>
+  <si>
+    <t>DigiKey</t>
+  </si>
+  <si>
+    <t>68021-410HLF</t>
   </si>
 </sst>
 </file>
@@ -886,12 +902,12 @@
   <dimension ref="A1:K200"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="35.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="46.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.28515625" style="10" customWidth="1"/>
     <col min="3" max="3" width="15.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.28515625" style="3" customWidth="1"/>
@@ -921,7 +937,7 @@
         <v>4</v>
       </c>
       <c r="K1" s="9">
-        <v>500</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="15" x14ac:dyDescent="0.25">
@@ -958,7 +974,7 @@
       </c>
       <c r="B4" s="14">
         <f>SUM(I6:I200)</f>
-        <v>0</v>
+        <v>35.769999999999996</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
@@ -1006,39 +1022,67 @@
       </c>
     </row>
     <row r="6" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="21"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="15"/>
+      <c r="A6" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="17">
+        <v>3087</v>
+      </c>
+      <c r="F6" s="15">
+        <v>1</v>
+      </c>
       <c r="G6" s="25">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>0</v>
-      </c>
-      <c r="H6" s="18"/>
+        <v>100</v>
+      </c>
+      <c r="H6" s="18">
+        <v>0.19989999999999999</v>
+      </c>
       <c r="I6" s="24">
         <f>SUM(H6*G6)</f>
-        <v>0</v>
+        <v>19.989999999999998</v>
       </c>
       <c r="J6" s="19"/>
       <c r="K6" s="19"/>
     </row>
     <row r="7" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="21"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="15"/>
+      <c r="A7" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="17">
+        <v>881</v>
+      </c>
+      <c r="F7" s="15">
+        <v>1</v>
+      </c>
       <c r="G7" s="25">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>0</v>
-      </c>
-      <c r="H7" s="18"/>
+        <v>100</v>
+      </c>
+      <c r="H7" s="18">
+        <v>0.1578</v>
+      </c>
       <c r="I7" s="24">
         <f>SUM(H7*G7)</f>
-        <v>0</v>
+        <v>15.78</v>
       </c>
       <c r="J7" s="19"/>
       <c r="K7" s="19"/>
@@ -1064,7 +1108,7 @@
     </row>
     <row r="9" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="21"/>
-      <c r="B9" s="20"/>
+      <c r="B9" s="22"/>
       <c r="C9" s="23"/>
       <c r="D9" s="19"/>
       <c r="E9" s="17"/>
@@ -4717,35 +4761,13 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A2:I2" r:id="rId1" display=" Projects and Stuff LLC - http://ww.projectsandstuff.com"/>
+    <hyperlink ref="B6" r:id="rId2"/>
+    <hyperlink ref="B7" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId4"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>